<commit_message>
LE0704: Escaleta y esqueleto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion04/Escaleta_LE_07_04_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion04/Escaleta_LE_07_04_CO.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
-    <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
+    <sheet name="DATOS" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -560,6 +561,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Edipo rey</t>
@@ -575,6 +577,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Antígona </t>
@@ -693,6 +696,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Don Juan Tenorio</t>
@@ -1065,6 +1069,7 @@
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1088,6 +1093,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1594,13 +1600,33 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1627,26 +1653,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="201">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1853,6 +1859,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2145,126 +2156,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="R41" sqref="R41"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="19.5" style="15" customWidth="1"/>
-    <col min="7" max="7" width="47.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="47.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="15" customWidth="1"/>
     <col min="9" max="9" width="11" style="15" customWidth="1"/>
-    <col min="10" max="10" width="37.5" customWidth="1"/>
-    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="18.5" customWidth="1"/>
-    <col min="15" max="15" width="37.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" style="15" customWidth="1"/>
     <col min="16" max="16" width="14" style="15" customWidth="1"/>
-    <col min="17" max="17" width="20.5" style="15" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" style="15" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.6640625" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="33.75" customHeight="1">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="M1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="43"/>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="47" t="s">
+      <c r="T1" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="44" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A2" s="38"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="39"/>
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="50"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="51"/>
       <c r="M2" s="12" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="46"/>
-    </row>
-    <row r="3" spans="1:21" ht="42">
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="44"/>
+    </row>
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
@@ -2321,7 +2332,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="42">
+    <row r="4" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -2378,7 +2389,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="28">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2435,7 +2446,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="70">
+    <row r="6" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -2492,7 +2503,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="28">
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -2549,7 +2560,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="98">
+    <row r="8" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
@@ -2606,7 +2617,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15">
+    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
@@ -2663,7 +2674,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="28">
+    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -2722,7 +2733,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15">
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
@@ -2783,7 +2794,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15">
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
@@ -2842,7 +2853,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15">
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
@@ -2901,7 +2912,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15">
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -2960,7 +2971,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15">
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
@@ -3021,7 +3032,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15">
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>16</v>
       </c>
@@ -3080,7 +3091,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15">
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
@@ -3139,7 +3150,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15">
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
@@ -3196,7 +3207,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="56">
+    <row r="19" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
@@ -3257,7 +3268,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="42">
+    <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>16</v>
       </c>
@@ -3316,7 +3327,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="98">
+    <row r="21" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
@@ -3373,7 +3384,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15">
+    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>16</v>
       </c>
@@ -3430,7 +3441,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="28">
+    <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>16</v>
       </c>
@@ -3489,7 +3500,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15">
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>16</v>
       </c>
@@ -3544,7 +3555,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15">
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>16</v>
       </c>
@@ -3599,7 +3610,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15">
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>16</v>
       </c>
@@ -3656,7 +3667,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="98">
+    <row r="27" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>16</v>
       </c>
@@ -3715,7 +3726,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="70">
+    <row r="28" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>16</v>
       </c>
@@ -3774,7 +3785,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="70">
+    <row r="29" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>16</v>
       </c>
@@ -3837,7 +3848,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="70">
+    <row r="30" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>16</v>
       </c>
@@ -3896,7 +3907,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="112">
+    <row r="31" spans="1:21" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>16</v>
       </c>
@@ -3955,7 +3966,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="84">
+    <row r="32" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>16</v>
       </c>
@@ -4014,7 +4025,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="56">
+    <row r="33" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>16</v>
       </c>
@@ -4077,7 +4088,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="70">
+    <row r="34" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>16</v>
       </c>
@@ -4136,7 +4147,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="28">
+    <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>16</v>
       </c>
@@ -4195,7 +4206,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="98">
+    <row r="36" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>16</v>
       </c>
@@ -4240,23 +4251,23 @@
       <c r="P36" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="Q36" s="49">
+      <c r="Q36" s="34">
         <v>6</v>
       </c>
-      <c r="R36" s="50" t="s">
+      <c r="R36" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="S36" s="51" t="s">
+      <c r="S36" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="T36" s="52" t="s">
+      <c r="T36" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="U36" s="51" t="s">
+      <c r="U36" s="36" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="15">
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>16</v>
       </c>
@@ -4311,7 +4322,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="15">
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>16</v>
       </c>
@@ -4368,7 +4379,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="70">
+    <row r="39" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>16</v>
       </c>
@@ -4427,7 +4438,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="42">
+    <row r="40" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>16</v>
       </c>
@@ -4482,7 +4493,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="112">
+    <row r="41" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>16</v>
       </c>
@@ -4541,7 +4552,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="42">
+    <row r="42" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>16</v>
       </c>
@@ -4596,7 +4607,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15">
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>16</v>
       </c>
@@ -4639,7 +4650,7 @@
       <c r="T43" s="7"/>
       <c r="U43" s="6"/>
     </row>
-    <row r="44" spans="1:21" ht="15">
+    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>16</v>
       </c>
@@ -4680,23 +4691,23 @@
       <c r="P44" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="Q44" s="53">
+      <c r="Q44" s="38">
         <v>6</v>
       </c>
-      <c r="R44" s="54" t="s">
+      <c r="R44" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="S44" s="55" t="s">
+      <c r="S44" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="T44" s="56" t="s">
+      <c r="T44" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="U44" s="55" t="s">
+      <c r="U44" s="40" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="15">
+    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>16</v>
       </c>
@@ -4751,218 +4762,212 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H46" s="29"/>
       <c r="P46" s="29"/>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H47" s="29"/>
       <c r="P47" s="29"/>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H48" s="29"/>
       <c r="P48" s="29"/>
     </row>
-    <row r="49" spans="8:16">
+    <row r="49" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H49" s="29"/>
       <c r="P49" s="29"/>
     </row>
-    <row r="50" spans="8:16">
+    <row r="50" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H50" s="29"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4977,79 +4982,16 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I8 I12:I14 I16:I19 I21:I22 I37:I40 I24:I28 I30 I32 I34:I35 I42:I45">
-      <formula1>$D$48:$D$49</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>DATOS!$E$14:$E$48</xm:f>
-          </x14:formula1>
-          <xm:sqref>N3:N42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>DATOS!$A$1:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>A3:A42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>DATOS!$D$1:$D$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>K3:K42 P3:P42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>DATOS!$B$1:$B$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>L3:L42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>DATOS!$E$1:$E$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>M3:M42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]DATOS!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>M43:M45</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]DATOS!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>L43:L45</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]DATOS!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>P43:P45 K43:K45</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]DATOS!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>A43:A45</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]DATOS!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>N43:N45</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -5065,27 +5007,27 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="16" customWidth="1"/>
     <col min="4" max="4" width="34" style="16" customWidth="1"/>
-    <col min="5" max="5" width="34.83203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="24.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="16" customWidth="1"/>
     <col min="7" max="7" width="18" style="16" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="16" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="16" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="16" customWidth="1"/>
     <col min="12" max="12" width="17" style="16" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="16"/>
-    <col min="14" max="14" width="24.33203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="69.83203125" style="16" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="16"/>
+    <col min="13" max="13" width="10.85546875" style="16"/>
+    <col min="14" max="14" width="24.28515625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="16" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="17" customFormat="1" ht="15">
+    <row r="1" spans="1:12" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
@@ -5102,7 +5044,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
@@ -5126,7 +5068,7 @@
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
     </row>
-    <row r="3" spans="1:12" ht="15">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
@@ -5145,7 +5087,7 @@
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
     </row>
-    <row r="4" spans="1:12" ht="15">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>18</v>
       </c>
@@ -5164,7 +5106,7 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
     </row>
-    <row r="5" spans="1:12" ht="15">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>9</v>
       </c>
@@ -5180,7 +5122,7 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
     </row>
-    <row r="6" spans="1:12" ht="15">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
@@ -5197,7 +5139,7 @@
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
     </row>
-    <row r="7" spans="1:12" ht="15">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>11</v>
       </c>
@@ -5214,7 +5156,7 @@
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
     </row>
-    <row r="8" spans="1:12" ht="15">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -5229,7 +5171,7 @@
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
     </row>
-    <row r="9" spans="1:12" ht="15">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -5244,7 +5186,7 @@
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
     </row>
-    <row r="10" spans="1:12" ht="15">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -5259,7 +5201,7 @@
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
     </row>
-    <row r="11" spans="1:12" ht="15">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -5274,7 +5216,7 @@
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
     </row>
-    <row r="12" spans="1:12" ht="15">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -5289,7 +5231,7 @@
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
     </row>
-    <row r="13" spans="1:12" ht="15">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -5304,7 +5246,7 @@
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
     </row>
-    <row r="14" spans="1:12" ht="15">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -5319,7 +5261,7 @@
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
     </row>
-    <row r="15" spans="1:12" ht="15">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -5334,7 +5276,7 @@
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
     </row>
-    <row r="16" spans="1:12" ht="15">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -5349,7 +5291,7 @@
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
     </row>
-    <row r="17" spans="2:12" ht="15">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="16" t="s">
@@ -5363,7 +5305,7 @@
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
     </row>
-    <row r="18" spans="2:12" ht="15">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="16" t="s">
@@ -5377,7 +5319,7 @@
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
     </row>
-    <row r="19" spans="2:12" ht="15">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="16" t="s">
@@ -5391,7 +5333,7 @@
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
     </row>
-    <row r="20" spans="2:12" ht="15">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="16" t="s">
@@ -5405,7 +5347,7 @@
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
     </row>
-    <row r="21" spans="2:12" ht="15">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -5420,7 +5362,7 @@
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
     </row>
-    <row r="22" spans="2:12" ht="15">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -5435,7 +5377,7 @@
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
     </row>
-    <row r="23" spans="2:12" ht="15">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -5450,7 +5392,7 @@
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
     </row>
-    <row r="24" spans="2:12" ht="15">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -5465,7 +5407,7 @@
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
     </row>
-    <row r="25" spans="2:12" ht="15">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -5480,7 +5422,7 @@
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
     </row>
-    <row r="26" spans="2:12" ht="15">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -5495,7 +5437,7 @@
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
     </row>
-    <row r="27" spans="2:12" ht="15">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -5510,7 +5452,7 @@
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
     </row>
-    <row r="28" spans="2:12" ht="15">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -5525,7 +5467,7 @@
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
     </row>
-    <row r="29" spans="2:12" ht="15">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -5540,7 +5482,7 @@
       <c r="K29" s="17"/>
       <c r="L29" s="17"/>
     </row>
-    <row r="30" spans="2:12" ht="15">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -5555,7 +5497,7 @@
       <c r="K30" s="17"/>
       <c r="L30" s="17"/>
     </row>
-    <row r="31" spans="2:12" ht="15">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -5570,7 +5512,7 @@
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
     </row>
-    <row r="32" spans="2:12" ht="15">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
@@ -5585,7 +5527,7 @@
       <c r="K32" s="17"/>
       <c r="L32" s="17"/>
     </row>
-    <row r="33" spans="2:12" ht="15">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -5600,7 +5542,7 @@
       <c r="K33" s="17"/>
       <c r="L33" s="17"/>
     </row>
-    <row r="34" spans="2:12" ht="15">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -5615,7 +5557,7 @@
       <c r="K34" s="17"/>
       <c r="L34" s="17"/>
     </row>
-    <row r="35" spans="2:12" ht="15">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
@@ -5630,7 +5572,7 @@
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
     </row>
-    <row r="36" spans="2:12" ht="15">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
@@ -5645,7 +5587,7 @@
       <c r="K36" s="17"/>
       <c r="L36" s="17"/>
     </row>
-    <row r="37" spans="2:12" ht="15">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -5660,7 +5602,7 @@
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
     </row>
-    <row r="38" spans="2:12" ht="15">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
@@ -5675,7 +5617,7 @@
       <c r="K38" s="17"/>
       <c r="L38" s="17"/>
     </row>
-    <row r="39" spans="2:12" ht="15">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -5690,7 +5632,7 @@
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
     </row>
-    <row r="40" spans="2:12" ht="15">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -5705,7 +5647,7 @@
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
     </row>
-    <row r="41" spans="2:12" ht="15">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -5720,7 +5662,7 @@
       <c r="K41" s="17"/>
       <c r="L41" s="17"/>
     </row>
-    <row r="42" spans="2:12" ht="15">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -5735,7 +5677,7 @@
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
     </row>
-    <row r="43" spans="2:12" ht="15">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
@@ -5750,7 +5692,7 @@
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
     </row>
-    <row r="44" spans="2:12" ht="15">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
@@ -5765,7 +5707,7 @@
       <c r="K44" s="17"/>
       <c r="L44" s="17"/>
     </row>
-    <row r="45" spans="2:12" ht="15">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
@@ -5780,7 +5722,7 @@
       <c r="K45" s="17"/>
       <c r="L45" s="17"/>
     </row>
-    <row r="46" spans="2:12" ht="15">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -5795,7 +5737,7 @@
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
     </row>
-    <row r="47" spans="2:12" ht="15">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -5810,7 +5752,7 @@
       <c r="K47" s="17"/>
       <c r="L47" s="17"/>
     </row>
-    <row r="48" spans="2:12" ht="15">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
@@ -5825,7 +5767,7 @@
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
     </row>
-    <row r="49" spans="2:12" ht="15">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -5837,7 +5779,7 @@
       <c r="K49" s="17"/>
       <c r="L49" s="17"/>
     </row>
-    <row r="50" spans="2:12" ht="15">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
@@ -5849,7 +5791,7 @@
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
     </row>
-    <row r="51" spans="2:12" ht="15">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
@@ -5862,7 +5804,7 @@
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
     </row>
-    <row r="52" spans="2:12" ht="15">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
@@ -5875,7 +5817,7 @@
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
     </row>
-    <row r="53" spans="2:12" ht="15">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
@@ -5888,7 +5830,7 @@
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
     </row>
-    <row r="54" spans="2:12" ht="15">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
@@ -5901,7 +5843,7 @@
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
     </row>
-    <row r="55" spans="2:12" ht="15">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
@@ -5914,7 +5856,7 @@
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
     </row>
-    <row r="56" spans="2:12" ht="15">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
@@ -5927,7 +5869,7 @@
       <c r="K56" s="17"/>
       <c r="L56" s="17"/>
     </row>
-    <row r="57" spans="2:12" ht="15">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
@@ -5940,7 +5882,7 @@
       <c r="K57" s="17"/>
       <c r="L57" s="17"/>
     </row>
-    <row r="58" spans="2:12" ht="15">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
       <c r="D58" s="17"/>
@@ -5953,7 +5895,7 @@
       <c r="K58" s="17"/>
       <c r="L58" s="17"/>
     </row>
-    <row r="59" spans="2:12" ht="15">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
       <c r="D59" s="17"/>
@@ -5966,7 +5908,7 @@
       <c r="K59" s="17"/>
       <c r="L59" s="17"/>
     </row>
-    <row r="60" spans="2:12" ht="15">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
       <c r="D60" s="17"/>
@@ -5979,7 +5921,7 @@
       <c r="K60" s="17"/>
       <c r="L60" s="17"/>
     </row>
-    <row r="61" spans="2:12" ht="15">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
       <c r="D61" s="17"/>
@@ -5992,7 +5934,7 @@
       <c r="K61" s="17"/>
       <c r="L61" s="17"/>
     </row>
-    <row r="62" spans="2:12" ht="15">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
@@ -6005,7 +5947,7 @@
       <c r="K62" s="17"/>
       <c r="L62" s="17"/>
     </row>
-    <row r="63" spans="2:12" ht="15">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
       <c r="D63" s="17"/>
@@ -6018,7 +5960,7 @@
       <c r="K63" s="17"/>
       <c r="L63" s="17"/>
     </row>
-    <row r="64" spans="2:12" ht="15">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
       <c r="D64" s="17"/>
@@ -6031,7 +5973,7 @@
       <c r="K64" s="17"/>
       <c r="L64" s="17"/>
     </row>
-    <row r="65" spans="1:12" ht="15">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
@@ -6044,7 +5986,7 @@
       <c r="K65" s="17"/>
       <c r="L65" s="17"/>
     </row>
-    <row r="66" spans="1:12" ht="15">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
       <c r="D66" s="17"/>
@@ -6057,7 +5999,7 @@
       <c r="K66" s="17"/>
       <c r="L66" s="17"/>
     </row>
-    <row r="67" spans="1:12" ht="15">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
       <c r="D67" s="17"/>
@@ -6070,7 +6012,7 @@
       <c r="K67" s="17"/>
       <c r="L67" s="17"/>
     </row>
-    <row r="68" spans="1:12" ht="15">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
       <c r="D68" s="17"/>
@@ -6083,7 +6025,7 @@
       <c r="K68" s="17"/>
       <c r="L68" s="17"/>
     </row>
-    <row r="69" spans="1:12" ht="15">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
       <c r="D69" s="17"/>
@@ -6096,7 +6038,7 @@
       <c r="K69" s="17"/>
       <c r="L69" s="17"/>
     </row>
-    <row r="70" spans="1:12" ht="15">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
       <c r="D70" s="17"/>
@@ -6109,7 +6051,7 @@
       <c r="K70" s="17"/>
       <c r="L70" s="17"/>
     </row>
-    <row r="71" spans="1:12" ht="15">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -6123,7 +6065,7 @@
       <c r="K71" s="17"/>
       <c r="L71" s="17"/>
     </row>
-    <row r="72" spans="1:12" ht="15">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="17"/>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -6137,7 +6079,7 @@
       <c r="K72" s="17"/>
       <c r="L72" s="17"/>
     </row>
-    <row r="73" spans="1:12" ht="15">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="17"/>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -6151,7 +6093,7 @@
       <c r="K73" s="17"/>
       <c r="L73" s="17"/>
     </row>
-    <row r="74" spans="1:12" ht="15">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
@@ -6165,7 +6107,7 @@
       <c r="K74" s="17"/>
       <c r="L74" s="17"/>
     </row>
-    <row r="75" spans="1:12" ht="15">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -6179,7 +6121,7 @@
       <c r="K75" s="17"/>
       <c r="L75" s="17"/>
     </row>
-    <row r="76" spans="1:12" ht="15">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -6193,7 +6135,7 @@
       <c r="K76" s="17"/>
       <c r="L76" s="17"/>
     </row>
-    <row r="77" spans="1:12" ht="15">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="17"/>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -6207,7 +6149,7 @@
       <c r="K77" s="17"/>
       <c r="L77" s="17"/>
     </row>
-    <row r="78" spans="1:12" ht="15">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="17"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
@@ -6221,7 +6163,7 @@
       <c r="K78" s="17"/>
       <c r="L78" s="17"/>
     </row>
-    <row r="79" spans="1:12" ht="15">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="17"/>
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
@@ -6235,7 +6177,7 @@
       <c r="K79" s="17"/>
       <c r="L79" s="17"/>
     </row>
-    <row r="80" spans="1:12" ht="15">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="17"/>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
@@ -6249,7 +6191,7 @@
       <c r="K80" s="17"/>
       <c r="L80" s="17"/>
     </row>
-    <row r="81" spans="1:12" ht="15">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="17"/>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -6263,7 +6205,7 @@
       <c r="K81" s="17"/>
       <c r="L81" s="17"/>
     </row>
-    <row r="82" spans="1:12" ht="15">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="17"/>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>
@@ -6277,7 +6219,7 @@
       <c r="K82" s="17"/>
       <c r="L82" s="17"/>
     </row>
-    <row r="83" spans="1:12" ht="15">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="17"/>
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
@@ -6291,7 +6233,7 @@
       <c r="K83" s="17"/>
       <c r="L83" s="17"/>
     </row>
-    <row r="84" spans="1:12" ht="15">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="17"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -6305,7 +6247,7 @@
       <c r="K84" s="17"/>
       <c r="L84" s="17"/>
     </row>
-    <row r="85" spans="1:12" ht="15">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="17"/>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -6319,7 +6261,7 @@
       <c r="K85" s="17"/>
       <c r="L85" s="17"/>
     </row>
-    <row r="86" spans="1:12" ht="15">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="17"/>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
@@ -6333,7 +6275,7 @@
       <c r="K86" s="17"/>
       <c r="L86" s="17"/>
     </row>
-    <row r="87" spans="1:12" ht="15">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="17"/>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -6347,7 +6289,7 @@
       <c r="K87" s="17"/>
       <c r="L87" s="17"/>
     </row>
-    <row r="88" spans="1:12" ht="15">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="17"/>
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
@@ -6361,7 +6303,7 @@
       <c r="K88" s="17"/>
       <c r="L88" s="17"/>
     </row>
-    <row r="89" spans="1:12" ht="15">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="17"/>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
@@ -6375,7 +6317,7 @@
       <c r="K89" s="17"/>
       <c r="L89" s="17"/>
     </row>
-    <row r="90" spans="1:12" ht="15">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="17"/>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
@@ -6389,7 +6331,7 @@
       <c r="K90" s="17"/>
       <c r="L90" s="17"/>
     </row>
-    <row r="91" spans="1:12" ht="15">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="17"/>
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
@@ -6403,7 +6345,7 @@
       <c r="K91" s="17"/>
       <c r="L91" s="17"/>
     </row>
-    <row r="92" spans="1:12" ht="15">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -6417,7 +6359,7 @@
       <c r="K92" s="17"/>
       <c r="L92" s="17"/>
     </row>
-    <row r="93" spans="1:12" ht="15">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="17"/>
       <c r="B93" s="17"/>
       <c r="C93" s="17"/>
@@ -6431,7 +6373,7 @@
       <c r="K93" s="17"/>
       <c r="L93" s="17"/>
     </row>
-    <row r="94" spans="1:12" ht="15">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="17"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -6445,7 +6387,7 @@
       <c r="K94" s="17"/>
       <c r="L94" s="17"/>
     </row>
-    <row r="95" spans="1:12" ht="15">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="17"/>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -6459,7 +6401,7 @@
       <c r="K95" s="17"/>
       <c r="L95" s="17"/>
     </row>
-    <row r="96" spans="1:12" ht="15">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="17"/>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
@@ -6473,7 +6415,7 @@
       <c r="K96" s="17"/>
       <c r="L96" s="17"/>
     </row>
-    <row r="97" spans="1:12" ht="15">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="17"/>
       <c r="B97" s="17"/>
       <c r="C97" s="17"/>
@@ -6487,7 +6429,7 @@
       <c r="K97" s="17"/>
       <c r="L97" s="17"/>
     </row>
-    <row r="98" spans="1:12" ht="15">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="17"/>
       <c r="B98" s="17"/>
       <c r="C98" s="17"/>
@@ -6501,7 +6443,7 @@
       <c r="K98" s="17"/>
       <c r="L98" s="17"/>
     </row>
-    <row r="99" spans="1:12" ht="15">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="17"/>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -6515,7 +6457,7 @@
       <c r="K99" s="17"/>
       <c r="L99" s="17"/>
     </row>
-    <row r="100" spans="1:12" ht="15">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
@@ -6529,7 +6471,7 @@
       <c r="K100" s="17"/>
       <c r="L100" s="17"/>
     </row>
-    <row r="101" spans="1:12" ht="15">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="17"/>
       <c r="B101" s="17"/>
       <c r="C101" s="17"/>
@@ -6543,7 +6485,7 @@
       <c r="K101" s="17"/>
       <c r="L101" s="17"/>
     </row>
-    <row r="102" spans="1:12" ht="15">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="17"/>
       <c r="B102" s="17"/>
       <c r="C102" s="17"/>
@@ -6557,7 +6499,7 @@
       <c r="K102" s="17"/>
       <c r="L102" s="17"/>
     </row>
-    <row r="103" spans="1:12" ht="15">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
       <c r="C103" s="17"/>
@@ -6571,7 +6513,7 @@
       <c r="K103" s="17"/>
       <c r="L103" s="17"/>
     </row>
-    <row r="104" spans="1:12" ht="15">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="17"/>
       <c r="B104" s="17"/>
       <c r="C104" s="17"/>
@@ -6585,7 +6527,7 @@
       <c r="K104" s="17"/>
       <c r="L104" s="17"/>
     </row>
-    <row r="105" spans="1:12" ht="15">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="17"/>
       <c r="B105" s="17"/>
       <c r="C105" s="17"/>
@@ -6599,7 +6541,7 @@
       <c r="K105" s="17"/>
       <c r="L105" s="17"/>
     </row>
-    <row r="106" spans="1:12" ht="15">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="17"/>
       <c r="B106" s="17"/>
       <c r="C106" s="17"/>
@@ -6613,7 +6555,7 @@
       <c r="K106" s="17"/>
       <c r="L106" s="17"/>
     </row>
-    <row r="107" spans="1:12" ht="15">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="17"/>
       <c r="B107" s="17"/>
       <c r="C107" s="17"/>
@@ -6627,7 +6569,7 @@
       <c r="K107" s="17"/>
       <c r="L107" s="17"/>
     </row>
-    <row r="108" spans="1:12" ht="15">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="17"/>
       <c r="B108" s="17"/>
       <c r="C108" s="17"/>
@@ -6641,7 +6583,7 @@
       <c r="K108" s="17"/>
       <c r="L108" s="17"/>
     </row>
-    <row r="109" spans="1:12" ht="15">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="17"/>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
@@ -6655,7 +6597,7 @@
       <c r="K109" s="17"/>
       <c r="L109" s="17"/>
     </row>
-    <row r="110" spans="1:12" ht="15">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="17"/>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>
@@ -6669,7 +6611,7 @@
       <c r="K110" s="17"/>
       <c r="L110" s="17"/>
     </row>
-    <row r="111" spans="1:12" ht="15">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="17"/>
       <c r="B111" s="17"/>
       <c r="C111" s="17"/>
@@ -6683,7 +6625,7 @@
       <c r="K111" s="17"/>
       <c r="L111" s="17"/>
     </row>
-    <row r="112" spans="1:12" ht="15">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="17"/>
       <c r="B112" s="17"/>
       <c r="C112" s="17"/>
@@ -6697,7 +6639,7 @@
       <c r="K112" s="17"/>
       <c r="L112" s="17"/>
     </row>
-    <row r="113" spans="1:12" ht="15">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
@@ -6711,7 +6653,7 @@
       <c r="K113" s="17"/>
       <c r="L113" s="17"/>
     </row>
-    <row r="114" spans="1:12" ht="15">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="17"/>
       <c r="B114" s="17"/>
       <c r="C114" s="17"/>
@@ -6725,7 +6667,7 @@
       <c r="K114" s="17"/>
       <c r="L114" s="17"/>
     </row>
-    <row r="115" spans="1:12" ht="15">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="17"/>
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
@@ -6739,7 +6681,7 @@
       <c r="K115" s="17"/>
       <c r="L115" s="17"/>
     </row>
-    <row r="116" spans="1:12" ht="15">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="17"/>
       <c r="B116" s="17"/>
       <c r="C116" s="17"/>
@@ -6753,7 +6695,7 @@
       <c r="K116" s="17"/>
       <c r="L116" s="17"/>
     </row>
-    <row r="117" spans="1:12" ht="15">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="17"/>
@@ -6767,7 +6709,7 @@
       <c r="K117" s="17"/>
       <c r="L117" s="17"/>
     </row>
-    <row r="118" spans="1:12" ht="15">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="17"/>
       <c r="B118" s="17"/>
       <c r="C118" s="17"/>
@@ -6781,7 +6723,7 @@
       <c r="K118" s="17"/>
       <c r="L118" s="17"/>
     </row>
-    <row r="119" spans="1:12" ht="15">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="17"/>
       <c r="B119" s="17"/>
       <c r="C119" s="17"/>
@@ -6795,7 +6737,7 @@
       <c r="K119" s="17"/>
       <c r="L119" s="17"/>
     </row>
-    <row r="120" spans="1:12" ht="15">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="17"/>
       <c r="B120" s="17"/>
       <c r="C120" s="17"/>
@@ -6809,7 +6751,7 @@
       <c r="K120" s="17"/>
       <c r="L120" s="17"/>
     </row>
-    <row r="121" spans="1:12" ht="15">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="17"/>
       <c r="B121" s="17"/>
       <c r="C121" s="17"/>
@@ -6823,7 +6765,7 @@
       <c r="K121" s="17"/>
       <c r="L121" s="17"/>
     </row>
-    <row r="122" spans="1:12" ht="15">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="17"/>
       <c r="B122" s="17"/>
       <c r="C122" s="17"/>
@@ -6837,7 +6779,7 @@
       <c r="K122" s="17"/>
       <c r="L122" s="17"/>
     </row>
-    <row r="123" spans="1:12" ht="15">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="17"/>
       <c r="B123" s="17"/>
       <c r="C123" s="17"/>
@@ -6851,7 +6793,7 @@
       <c r="K123" s="17"/>
       <c r="L123" s="17"/>
     </row>
-    <row r="124" spans="1:12" ht="15">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="17"/>
       <c r="B124" s="17"/>
       <c r="C124" s="17"/>
@@ -6865,7 +6807,7 @@
       <c r="K124" s="17"/>
       <c r="L124" s="17"/>
     </row>
-    <row r="125" spans="1:12" ht="15">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="17"/>
       <c r="B125" s="17"/>
       <c r="C125" s="17"/>
@@ -6879,7 +6821,7 @@
       <c r="K125" s="17"/>
       <c r="L125" s="17"/>
     </row>
-    <row r="126" spans="1:12" ht="15">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="17"/>
       <c r="B126" s="17"/>
       <c r="C126" s="17"/>
@@ -6893,7 +6835,7 @@
       <c r="K126" s="17"/>
       <c r="L126" s="17"/>
     </row>
-    <row r="127" spans="1:12" ht="15">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="17"/>
       <c r="B127" s="17"/>
       <c r="C127" s="17"/>
@@ -6907,7 +6849,7 @@
       <c r="K127" s="17"/>
       <c r="L127" s="17"/>
     </row>
-    <row r="128" spans="1:12" ht="15">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="17"/>
       <c r="B128" s="17"/>
       <c r="C128" s="17"/>
@@ -6921,7 +6863,7 @@
       <c r="K128" s="17"/>
       <c r="L128" s="17"/>
     </row>
-    <row r="129" spans="1:12" ht="15">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="17"/>
       <c r="B129" s="17"/>
       <c r="C129" s="17"/>
@@ -6935,7 +6877,7 @@
       <c r="K129" s="17"/>
       <c r="L129" s="17"/>
     </row>
-    <row r="130" spans="1:12" ht="15">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="17"/>
       <c r="B130" s="17"/>
       <c r="C130" s="17"/>
@@ -6949,7 +6891,7 @@
       <c r="K130" s="17"/>
       <c r="L130" s="17"/>
     </row>
-    <row r="131" spans="1:12" ht="15">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="17"/>
       <c r="B131" s="17"/>
       <c r="C131" s="17"/>
@@ -6963,7 +6905,7 @@
       <c r="K131" s="17"/>
       <c r="L131" s="17"/>
     </row>
-    <row r="132" spans="1:12" ht="15">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="17"/>
       <c r="B132" s="17"/>
       <c r="C132" s="17"/>
@@ -6977,7 +6919,7 @@
       <c r="K132" s="17"/>
       <c r="L132" s="17"/>
     </row>
-    <row r="133" spans="1:12" ht="15">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="17"/>
       <c r="B133" s="17"/>
       <c r="C133" s="17"/>

</xml_diff>